<commit_message>
Try to publish all of nicam16-7s.
</commit_message>
<xml_diff>
--- a/cmip6/models/nicam16-7s/cmip6_miroc_nicam16-7s_toplevel.xlsx
+++ b/cmip6/models/nicam16-7s/cmip6_miroc_nicam16-7s_toplevel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Takahiro\Google ドライブ\2018 統合\ES-DOC\test\cmip6\models\nicam16-7s\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="2. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="3. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="448">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1349,17 +1354,34 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>[Tentative] Team NICAM within Team MIROC</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>NICAM</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Non-hydrostatic high resolution cloud resolving global atmospheric model</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Non-hydrostatic cloud resolving non-parametric
+Icosahedral grid</t>
+    <phoneticPr fontId="13"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1442,6 +1464,13 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1531,15 +1560,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1581,7 +1618,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1613,9 +1650,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1647,6 +1685,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1822,24 +1861,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.75" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +1888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="23.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1855,7 +1896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="23.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1863,7 +1904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="23.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1871,7 +1912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1879,17 +1920,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="23.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="23.25">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="23.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1897,7 +1938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="23.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1905,7 +1946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="23.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1914,6 +1955,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="13"/>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>
     <hyperlink ref="B13" r:id="rId2"/>
@@ -1923,19 +1965,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="200.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="200.75" customWidth="1"/>
+    <col min="3" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1943,7 +1987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
@@ -1951,7 +1995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1964,10 +2008,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:2">
+    <row r="6" spans="1:2" ht="18">
+      <c r="B6" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -1975,7 +2021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -1988,26 +2034,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD240"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH240"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="200.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="200.75" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -2043,7 +2092,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -2070,7 +2121,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="7" t="s">
@@ -2096,8 +2149,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B16" s="11" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="A19" s="12" t="s">
@@ -2136,7 +2191,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
+    <row r="25" spans="1:3" ht="177.95" customHeight="1">
       <c r="B25" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
@@ -2242,7 +2297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
+    <row r="46" spans="1:3" ht="177.95" customHeight="1">
       <c r="B46" s="11"/>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -2589,7 +2644,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="178" customHeight="1">
+    <row r="108" spans="1:3" ht="177.95" customHeight="1">
       <c r="B108" s="11"/>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
@@ -2789,7 +2844,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="178" customHeight="1">
+    <row r="148" spans="1:3" ht="177.95" customHeight="1">
       <c r="B148" s="11"/>
     </row>
     <row r="150" spans="1:3" ht="24" customHeight="1">
@@ -2816,7 +2871,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="178" customHeight="1">
+    <row r="153" spans="1:3" ht="177.95" customHeight="1">
       <c r="B153" s="11"/>
     </row>
     <row r="155" spans="1:3" ht="24" customHeight="1">
@@ -2843,7 +2898,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="178" customHeight="1">
+    <row r="158" spans="1:3" ht="177.95" customHeight="1">
       <c r="B158" s="11"/>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
@@ -2870,7 +2925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="178" customHeight="1">
+    <row r="163" spans="1:3" ht="177.95" customHeight="1">
       <c r="B163" s="11"/>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
@@ -2897,7 +2952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="178" customHeight="1">
+    <row r="168" spans="1:3" ht="177.95" customHeight="1">
       <c r="B168" s="11"/>
     </row>
     <row r="170" spans="1:3" ht="24" customHeight="1">
@@ -2924,7 +2979,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="178" customHeight="1">
+    <row r="173" spans="1:3" ht="177.95" customHeight="1">
       <c r="B173" s="11"/>
     </row>
     <row r="176" spans="1:3" ht="24" customHeight="1">
@@ -2964,7 +3019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="178" customHeight="1">
+    <row r="182" spans="1:3" ht="177.95" customHeight="1">
       <c r="B182" s="11"/>
     </row>
     <row r="184" spans="1:3" ht="24" customHeight="1">
@@ -2991,7 +3046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="178" customHeight="1">
+    <row r="187" spans="1:3" ht="177.95" customHeight="1">
       <c r="B187" s="11"/>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
@@ -3018,7 +3073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="178" customHeight="1">
+    <row r="192" spans="1:3" ht="177.95" customHeight="1">
       <c r="B192" s="11"/>
     </row>
     <row r="194" spans="1:3" ht="24" customHeight="1">
@@ -3045,7 +3100,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="178" customHeight="1">
+    <row r="197" spans="1:3" ht="177.95" customHeight="1">
       <c r="B197" s="11"/>
     </row>
     <row r="199" spans="1:3" ht="24" customHeight="1">
@@ -3072,7 +3127,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="178" customHeight="1">
+    <row r="202" spans="1:3" ht="177.95" customHeight="1">
       <c r="B202" s="11"/>
     </row>
     <row r="204" spans="1:3" ht="24" customHeight="1">
@@ -3099,7 +3154,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="178" customHeight="1">
+    <row r="207" spans="1:3" ht="177.95" customHeight="1">
       <c r="B207" s="11"/>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
@@ -3126,7 +3181,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="178" customHeight="1">
+    <row r="212" spans="1:3" ht="177.95" customHeight="1">
       <c r="B212" s="11"/>
     </row>
     <row r="214" spans="1:3" ht="24" customHeight="1">
@@ -3153,7 +3208,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="178" customHeight="1">
+    <row r="217" spans="1:3" ht="177.95" customHeight="1">
       <c r="B217" s="11"/>
     </row>
     <row r="219" spans="1:3" ht="24" customHeight="1">
@@ -3180,7 +3235,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="178" customHeight="1">
+    <row r="222" spans="1:3" ht="177.95" customHeight="1">
       <c r="B222" s="11"/>
     </row>
     <row r="225" spans="1:3" ht="24" customHeight="1">
@@ -3220,7 +3275,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="178" customHeight="1">
+    <row r="231" spans="1:3" ht="177.95" customHeight="1">
       <c r="B231" s="11"/>
     </row>
     <row r="234" spans="1:3" ht="24" customHeight="1">
@@ -3260,10 +3315,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="178" customHeight="1">
+    <row r="240" spans="1:3" ht="177.95" customHeight="1">
       <c r="B240" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="13"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
       <formula1>AA75:AH75</formula1>
@@ -3283,17 +3339,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD323"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG323"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="200.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="200.75" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -3355,7 +3411,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -3478,7 +3534,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="178" customHeight="1">
+    <row r="33" spans="1:33" ht="177.95" customHeight="1">
       <c r="B33" s="11"/>
     </row>
     <row r="36" spans="1:33" ht="24" customHeight="1">
@@ -3566,7 +3622,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="178" customHeight="1">
+    <row r="47" spans="1:33" ht="177.95" customHeight="1">
       <c r="B47" s="11"/>
     </row>
     <row r="50" spans="1:33" ht="24" customHeight="1">
@@ -3654,7 +3710,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="178" customHeight="1">
+    <row r="61" spans="1:33" ht="177.95" customHeight="1">
       <c r="B61" s="11"/>
     </row>
     <row r="64" spans="1:33" ht="24" customHeight="1">
@@ -3742,7 +3798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="178" customHeight="1">
+    <row r="75" spans="1:33" ht="177.95" customHeight="1">
       <c r="B75" s="11"/>
     </row>
     <row r="78" spans="1:33" ht="24" customHeight="1">
@@ -3830,7 +3886,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="178" customHeight="1">
+    <row r="89" spans="1:33" ht="177.95" customHeight="1">
       <c r="B89" s="11"/>
     </row>
     <row r="92" spans="1:33" ht="24" customHeight="1">
@@ -3955,7 +4011,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:33" ht="178" customHeight="1">
+    <row r="107" spans="1:33" ht="177.95" customHeight="1">
       <c r="B107" s="11"/>
     </row>
     <row r="110" spans="1:33" ht="24" customHeight="1">
@@ -4078,7 +4134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:33" ht="178" customHeight="1">
+    <row r="129" spans="1:33" ht="177.95" customHeight="1">
       <c r="B129" s="11"/>
     </row>
     <row r="132" spans="1:33" ht="24" customHeight="1">
@@ -4166,7 +4222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="143" spans="1:33" ht="178" customHeight="1">
+    <row r="143" spans="1:33" ht="177.95" customHeight="1">
       <c r="B143" s="11"/>
     </row>
     <row r="146" spans="1:33" ht="24" customHeight="1">
@@ -4254,7 +4310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:33" ht="178" customHeight="1">
+    <row r="157" spans="1:33" ht="177.95" customHeight="1">
       <c r="B157" s="11"/>
     </row>
     <row r="160" spans="1:33" ht="24" customHeight="1">
@@ -4342,7 +4398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:33" ht="178" customHeight="1">
+    <row r="171" spans="1:33" ht="177.95" customHeight="1">
       <c r="B171" s="11"/>
     </row>
     <row r="174" spans="1:33" ht="24" customHeight="1">
@@ -4452,7 +4508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="189" spans="1:33" ht="178" customHeight="1">
+    <row r="189" spans="1:33" ht="177.95" customHeight="1">
       <c r="B189" s="11"/>
     </row>
     <row r="192" spans="1:33" ht="24" customHeight="1">
@@ -4584,7 +4640,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="211" spans="1:33" ht="178" customHeight="1">
+    <row r="211" spans="1:33" ht="177.95" customHeight="1">
       <c r="B211" s="11"/>
     </row>
     <row r="214" spans="1:33" ht="24" customHeight="1">
@@ -4672,7 +4728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="225" spans="1:33" ht="178" customHeight="1">
+    <row r="225" spans="1:33" ht="177.95" customHeight="1">
       <c r="B225" s="11"/>
     </row>
     <row r="228" spans="1:33" ht="24" customHeight="1">
@@ -4840,7 +4896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="247" spans="1:33" ht="178" customHeight="1">
+    <row r="247" spans="1:33" ht="177.95" customHeight="1">
       <c r="B247" s="11"/>
     </row>
     <row r="250" spans="1:33" ht="24" customHeight="1">
@@ -5008,7 +5064,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="269" spans="1:32" ht="178" customHeight="1">
+    <row r="269" spans="1:32" ht="177.95" customHeight="1">
       <c r="B269" s="11"/>
     </row>
     <row r="272" spans="1:32" ht="24" customHeight="1">
@@ -5096,7 +5152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="283" spans="1:33" ht="178" customHeight="1">
+    <row r="283" spans="1:33" ht="177.95" customHeight="1">
       <c r="B283" s="11"/>
     </row>
     <row r="286" spans="1:33" ht="24" customHeight="1">
@@ -5241,7 +5297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="309" spans="1:32" ht="178" customHeight="1">
+    <row r="309" spans="1:32" ht="177.95" customHeight="1">
       <c r="B309" s="11"/>
     </row>
     <row r="312" spans="1:32" ht="24" customHeight="1">
@@ -5326,10 +5382,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="178" customHeight="1">
+    <row r="323" spans="1:3" ht="177.95" customHeight="1">
       <c r="B323" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="13"/>
   <dataValidations count="27">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
       <formula1>AA28:AG28</formula1>
@@ -5414,5 +5471,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>